<commit_message>
Updated template with more exclusions
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS/Data/KPITemplateV4.6.xlsx
+++ b/Projects/CCBOTTLERSUS/Data/KPITemplateV4.6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,6 +20,7 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$I$63</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Survey!$A$1:$E$28</definedName>
   </definedNames>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="284">
   <si>
     <t xml:space="preserve">Region</t>
   </si>
@@ -837,6 +838,9 @@
   </si>
   <si>
     <t xml:space="preserve">product_ean_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GENERAL COFFEE OTHER, GENERAL DAIRY OTHER, GENERAL ENERGY OTHER, GENERAL ISOTONIC OTHER, GENERAL JC/DR SHELF STABLE OTHER, GENERAL SSD OTHER, GENERAL WATER OTHER, Juice Other, Tea Other</t>
   </si>
   <si>
     <t xml:space="preserve">53, 4587, 4900002826, 4900003165, 4900000978</t>
@@ -1022,7 +1026,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1075,10 +1079,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1096,10 +1096,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1133,10 +1129,6 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1234,18 +1226,18 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.3886639676113"/>
@@ -1402,7 +1394,7 @@
       </c>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" s="5" customFormat="true" ht="100.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="100.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1412,7 +1404,7 @@
       <c r="C5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="0"/>
+      <c r="E5" s="5"/>
       <c r="F5" s="4" t="s">
         <v>31</v>
       </c>
@@ -1425,17 +1417,16 @@
       <c r="I5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="K5" s="0"/>
+      <c r="J5" s="5"/>
       <c r="L5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="0"/>
       <c r="O5" s="4" t="n">
         <v>25</v>
       </c>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" s="5" customFormat="true" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -1445,7 +1436,6 @@
       <c r="C6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="0"/>
       <c r="E6" s="4" t="s">
         <v>35</v>
       </c>
@@ -1461,17 +1451,16 @@
       <c r="I6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="0"/>
+      <c r="J6" s="5"/>
       <c r="L6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="0"/>
       <c r="O6" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" s="5" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1481,7 +1470,6 @@
       <c r="C7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="0"/>
       <c r="E7" s="4" t="s">
         <v>35</v>
       </c>
@@ -1497,17 +1485,16 @@
       <c r="I7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="0"/>
+      <c r="J7" s="5"/>
       <c r="L7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M7" s="0"/>
       <c r="O7" s="4" t="n">
         <v>10</v>
       </c>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" s="5" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -1517,7 +1504,6 @@
       <c r="C8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="0"/>
       <c r="E8" s="4" t="s">
         <v>35</v>
       </c>
@@ -1533,17 +1519,16 @@
       <c r="I8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="0"/>
+      <c r="J8" s="5"/>
       <c r="L8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M8" s="0"/>
       <c r="O8" s="4" t="n">
         <v>10</v>
       </c>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" s="5" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -1553,8 +1538,6 @@
       <c r="C9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="0"/>
-      <c r="E9" s="0"/>
       <c r="F9" s="4" t="s">
         <v>43</v>
       </c>
@@ -1567,17 +1550,16 @@
       <c r="I9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="0"/>
+      <c r="J9" s="5"/>
       <c r="L9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="0"/>
       <c r="O9" s="4" t="n">
         <v>10</v>
       </c>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" s="5" customFormat="true" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1587,8 +1569,6 @@
       <c r="C10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="0"/>
-      <c r="E10" s="0"/>
       <c r="F10" s="4" t="s">
         <v>45</v>
       </c>
@@ -1601,17 +1581,16 @@
       <c r="I10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="0"/>
+      <c r="J10" s="5"/>
       <c r="L10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M10" s="0"/>
       <c r="O10" s="4" t="n">
         <v>10</v>
       </c>
       <c r="P10" s="4"/>
     </row>
-    <row r="11" s="5" customFormat="true" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -1621,8 +1600,6 @@
       <c r="C11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="0"/>
-      <c r="E11" s="0"/>
       <c r="F11" s="4" t="s">
         <v>47</v>
       </c>
@@ -1635,17 +1612,16 @@
       <c r="I11" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="K11" s="0"/>
+      <c r="J11" s="5"/>
       <c r="L11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M11" s="0"/>
       <c r="O11" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P11" s="4"/>
     </row>
-    <row r="12" s="5" customFormat="true" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1655,8 +1631,6 @@
       <c r="C12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="0"/>
-      <c r="E12" s="0"/>
       <c r="F12" s="4" t="s">
         <v>49</v>
       </c>
@@ -1669,17 +1643,16 @@
       <c r="I12" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="K12" s="0"/>
+      <c r="J12" s="5"/>
       <c r="L12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M12" s="0"/>
       <c r="O12" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" s="5" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -1698,7 +1671,6 @@
       <c r="F13" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="0"/>
       <c r="H13" s="4" t="s">
         <v>50</v>
       </c>
@@ -1708,17 +1680,15 @@
       <c r="J13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K13" s="0"/>
       <c r="L13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M13" s="0"/>
       <c r="O13" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P13" s="4"/>
     </row>
-    <row r="14" s="5" customFormat="true" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
@@ -1737,7 +1707,6 @@
       <c r="F14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="0"/>
       <c r="H14" s="4" t="s">
         <v>52</v>
       </c>
@@ -1747,7 +1716,6 @@
       <c r="J14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="0"/>
       <c r="L14" s="4" t="s">
         <v>37</v>
       </c>
@@ -1759,7 +1727,7 @@
       </c>
       <c r="P14" s="4"/>
     </row>
-    <row r="15" s="5" customFormat="true" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1772,19 +1740,15 @@
       <c r="D15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="0"/>
       <c r="F15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="0"/>
       <c r="H15" s="4" t="s">
         <v>54</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="0"/>
-      <c r="K15" s="0"/>
       <c r="L15" s="4" t="s">
         <v>57</v>
       </c>
@@ -1796,7 +1760,7 @@
       </c>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" s="5" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1806,8 +1770,6 @@
       <c r="C16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="0"/>
-      <c r="E16" s="0"/>
       <c r="F16" s="4" t="s">
         <v>59</v>
       </c>
@@ -1820,18 +1782,15 @@
       <c r="I16" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J16" s="0"/>
-      <c r="K16" s="0"/>
       <c r="L16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M16" s="0"/>
       <c r="O16" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P16" s="4"/>
     </row>
-    <row r="17" s="5" customFormat="true" ht="86.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="86.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -1841,8 +1800,6 @@
       <c r="C17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="0"/>
-      <c r="E17" s="0"/>
       <c r="F17" s="4" t="s">
         <v>61</v>
       </c>
@@ -1855,18 +1812,15 @@
       <c r="I17" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J17" s="0"/>
-      <c r="K17" s="0"/>
       <c r="L17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M17" s="0"/>
       <c r="O17" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P17" s="4"/>
     </row>
-    <row r="18" s="5" customFormat="true" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -1876,8 +1830,6 @@
       <c r="C18" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="0"/>
-      <c r="E18" s="0"/>
       <c r="F18" s="4" t="s">
         <v>63</v>
       </c>
@@ -1890,18 +1842,15 @@
       <c r="I18" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J18" s="0"/>
-      <c r="K18" s="0"/>
       <c r="L18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M18" s="0"/>
       <c r="O18" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P18" s="4"/>
     </row>
-    <row r="19" s="5" customFormat="true" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
@@ -1911,8 +1860,6 @@
       <c r="C19" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="0"/>
-      <c r="E19" s="0"/>
       <c r="F19" s="4" t="s">
         <v>65</v>
       </c>
@@ -1925,18 +1872,15 @@
       <c r="I19" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J19" s="0"/>
-      <c r="K19" s="0"/>
       <c r="L19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M19" s="0"/>
       <c r="O19" s="4" t="n">
         <v>10</v>
       </c>
       <c r="P19" s="4"/>
     </row>
-    <row r="20" s="5" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
@@ -1946,8 +1890,6 @@
       <c r="C20" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="0"/>
-      <c r="E20" s="0"/>
       <c r="F20" s="4" t="s">
         <v>67</v>
       </c>
@@ -1960,18 +1902,15 @@
       <c r="I20" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J20" s="0"/>
-      <c r="K20" s="0"/>
       <c r="L20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M20" s="0"/>
       <c r="O20" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P20" s="4"/>
     </row>
-    <row r="21" s="5" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -1981,8 +1920,6 @@
       <c r="C21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="0"/>
-      <c r="E21" s="0"/>
       <c r="F21" s="4" t="s">
         <v>69</v>
       </c>
@@ -1995,18 +1932,15 @@
       <c r="I21" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J21" s="0"/>
-      <c r="K21" s="0"/>
       <c r="L21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M21" s="0"/>
       <c r="O21" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P21" s="4"/>
     </row>
-    <row r="22" s="5" customFormat="true" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
         <v>16</v>
       </c>
@@ -2016,8 +1950,6 @@
       <c r="C22" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="0"/>
-      <c r="E22" s="0"/>
       <c r="F22" s="4" t="s">
         <v>71</v>
       </c>
@@ -2030,18 +1962,15 @@
       <c r="I22" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J22" s="0"/>
-      <c r="K22" s="0"/>
       <c r="L22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M22" s="0"/>
       <c r="O22" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" s="5" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
         <v>16</v>
       </c>
@@ -2051,8 +1980,6 @@
       <c r="C23" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="0"/>
-      <c r="E23" s="0"/>
       <c r="F23" s="4" t="s">
         <v>73</v>
       </c>
@@ -2065,18 +1992,15 @@
       <c r="I23" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J23" s="0"/>
-      <c r="K23" s="0"/>
       <c r="L23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M23" s="0"/>
       <c r="O23" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" s="5" customFormat="true" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>16</v>
       </c>
@@ -2086,14 +2010,12 @@
       <c r="C24" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="0"/>
       <c r="E24" s="4" t="s">
         <v>55</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G24" s="0"/>
       <c r="H24" s="4" t="s">
         <v>74</v>
       </c>
@@ -2103,7 +2025,6 @@
       <c r="J24" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K24" s="0"/>
       <c r="L24" s="4" t="s">
         <v>37</v>
       </c>
@@ -2115,7 +2036,7 @@
       </c>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" s="5" customFormat="true" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
         <v>16</v>
       </c>
@@ -2125,14 +2046,12 @@
       <c r="C25" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="0"/>
       <c r="E25" s="4" t="s">
         <v>55</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G25" s="0"/>
       <c r="H25" s="4" t="s">
         <v>76</v>
       </c>
@@ -2142,17 +2061,15 @@
       <c r="J25" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K25" s="0"/>
       <c r="L25" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M25" s="0"/>
       <c r="O25" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" s="5" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -2165,31 +2082,27 @@
       <c r="D26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="0"/>
       <c r="F26" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G26" s="0"/>
       <c r="H26" s="4" t="s">
         <v>78</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J26" s="0"/>
       <c r="K26" s="4" t="s">
         <v>80</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M26" s="0"/>
       <c r="O26" s="4" t="n">
         <v>10</v>
       </c>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" s="5" customFormat="true" ht="86.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="86.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
         <v>16</v>
       </c>
@@ -2202,30 +2115,26 @@
       <c r="D27" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="0"/>
       <c r="F27" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G27" s="0"/>
       <c r="H27" s="4" t="s">
         <v>22</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J27" s="0"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M27" s="0"/>
       <c r="O27" s="4" t="n">
         <v>30</v>
       </c>
       <c r="P27" s="4"/>
       <c r="Q27" s="6"/>
     </row>
-    <row r="28" s="5" customFormat="true" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
         <v>16</v>
       </c>
@@ -2238,30 +2147,24 @@
       <c r="D28" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E28" s="0"/>
       <c r="F28" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G28" s="0"/>
       <c r="H28" s="4" t="s">
         <v>83</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J28" s="0"/>
-      <c r="K28" s="0"/>
       <c r="L28" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M28" s="0"/>
       <c r="O28" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P28" s="4"/>
-      <c r="Q28" s="0"/>
-    </row>
-    <row r="29" s="5" customFormat="true" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="29" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
@@ -2274,11 +2177,9 @@
       <c r="D29" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="0"/>
       <c r="F29" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G29" s="0"/>
       <c r="H29" s="4" t="s">
         <v>85</v>
       </c>
@@ -2288,7 +2189,6 @@
       <c r="J29" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K29" s="0"/>
       <c r="L29" s="4" t="s">
         <v>37</v>
       </c>
@@ -2299,9 +2199,8 @@
         <v>5</v>
       </c>
       <c r="P29" s="4"/>
-      <c r="Q29" s="0"/>
-    </row>
-    <row r="30" s="5" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="30" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
         <v>16</v>
       </c>
@@ -2314,30 +2213,25 @@
       <c r="D30" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="0"/>
       <c r="F30" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G30" s="0"/>
       <c r="H30" s="4" t="s">
         <v>80</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J30" s="0"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M30" s="0"/>
       <c r="O30" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P30" s="4"/>
-      <c r="Q30" s="0"/>
-    </row>
-    <row r="31" s="5" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="31" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
         <v>16</v>
       </c>
@@ -2350,32 +2244,27 @@
       <c r="D31" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E31" s="0"/>
       <c r="F31" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G31" s="0"/>
       <c r="H31" s="4" t="s">
         <v>88</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J31" s="0"/>
       <c r="K31" s="4" t="s">
         <v>80</v>
       </c>
       <c r="L31" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M31" s="0"/>
       <c r="O31" s="4" t="n">
         <v>10</v>
       </c>
       <c r="P31" s="4"/>
-      <c r="Q31" s="0"/>
-    </row>
-    <row r="32" s="5" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="32" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
         <v>16</v>
       </c>
@@ -2388,30 +2277,24 @@
       <c r="D32" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E32" s="0"/>
       <c r="F32" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G32" s="0"/>
       <c r="H32" s="4" t="s">
         <v>90</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J32" s="0"/>
-      <c r="K32" s="0"/>
       <c r="L32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M32" s="0"/>
       <c r="O32" s="4" t="n">
         <v>20</v>
       </c>
       <c r="P32" s="4"/>
-      <c r="Q32" s="0"/>
-    </row>
-    <row r="33" s="5" customFormat="true" ht="72.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="33" customFormat="false" ht="72.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
@@ -2428,15 +2311,12 @@
       <c r="F33" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G33" s="0"/>
       <c r="H33" s="4" t="s">
         <v>93</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J33" s="0"/>
-      <c r="K33" s="0"/>
       <c r="L33" s="4" t="s">
         <v>23</v>
       </c>
@@ -2447,9 +2327,8 @@
         <v>10</v>
       </c>
       <c r="P33" s="4"/>
-      <c r="Q33" s="0"/>
-    </row>
-    <row r="34" s="5" customFormat="true" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="34" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
         <v>16</v>
       </c>
@@ -2462,19 +2341,15 @@
       <c r="D34" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E34" s="0"/>
       <c r="F34" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G34" s="0"/>
       <c r="H34" s="4" t="s">
         <v>97</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J34" s="0"/>
-      <c r="K34" s="0"/>
       <c r="L34" s="4" t="s">
         <v>23</v>
       </c>
@@ -2485,9 +2360,8 @@
         <v>20</v>
       </c>
       <c r="P34" s="4"/>
-      <c r="Q34" s="0"/>
-    </row>
-    <row r="35" s="5" customFormat="true" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="35" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
         <v>16</v>
       </c>
@@ -2497,8 +2371,6 @@
       <c r="C35" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D35" s="0"/>
-      <c r="E35" s="0"/>
       <c r="F35" s="4" t="s">
         <v>101</v>
       </c>
@@ -2511,19 +2383,15 @@
       <c r="I35" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J35" s="0"/>
-      <c r="K35" s="0"/>
       <c r="L35" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M35" s="0"/>
       <c r="O35" s="4" t="n">
         <v>10</v>
       </c>
       <c r="P35" s="4"/>
-      <c r="Q35" s="0"/>
-    </row>
-    <row r="36" s="5" customFormat="true" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="36" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
         <v>16</v>
       </c>
@@ -2533,8 +2401,6 @@
       <c r="C36" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D36" s="0"/>
-      <c r="E36" s="0"/>
       <c r="F36" s="4" t="s">
         <v>103</v>
       </c>
@@ -2547,19 +2413,16 @@
       <c r="I36" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J36" s="0"/>
-      <c r="K36" s="0"/>
       <c r="L36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M36" s="0"/>
       <c r="O36" s="4" t="n">
         <v>10</v>
       </c>
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
     </row>
-    <row r="37" s="5" customFormat="true" ht="100.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="100.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
         <v>16</v>
       </c>
@@ -2569,8 +2432,6 @@
       <c r="C37" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D37" s="0"/>
-      <c r="E37" s="0"/>
       <c r="F37" s="4" t="s">
         <v>31</v>
       </c>
@@ -2583,19 +2444,15 @@
       <c r="I37" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J37" s="0"/>
-      <c r="K37" s="0"/>
       <c r="L37" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M37" s="0"/>
       <c r="O37" s="4" t="n">
         <v>25</v>
       </c>
       <c r="P37" s="4"/>
-      <c r="Q37" s="0"/>
-    </row>
-    <row r="38" s="5" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="38" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
         <v>16</v>
       </c>
@@ -2605,8 +2462,6 @@
       <c r="C38" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D38" s="0"/>
-      <c r="E38" s="0"/>
       <c r="F38" s="4" t="s">
         <v>106</v>
       </c>
@@ -2619,19 +2474,15 @@
       <c r="I38" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J38" s="0"/>
-      <c r="K38" s="0"/>
       <c r="L38" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M38" s="0"/>
       <c r="O38" s="4" t="n">
         <v>10</v>
       </c>
       <c r="P38" s="4"/>
-      <c r="Q38" s="0"/>
-    </row>
-    <row r="39" s="5" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="39" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
         <v>16</v>
       </c>
@@ -2641,8 +2492,6 @@
       <c r="C39" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D39" s="0"/>
-      <c r="E39" s="0"/>
       <c r="F39" s="4" t="s">
         <v>108</v>
       </c>
@@ -2655,19 +2504,15 @@
       <c r="I39" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J39" s="0"/>
-      <c r="K39" s="0"/>
       <c r="L39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M39" s="0"/>
       <c r="O39" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P39" s="4"/>
-      <c r="Q39" s="0"/>
-    </row>
-    <row r="40" s="5" customFormat="true" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="40" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
         <v>16</v>
       </c>
@@ -2677,8 +2522,6 @@
       <c r="C40" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D40" s="0"/>
-      <c r="E40" s="0"/>
       <c r="F40" s="4" t="s">
         <v>110</v>
       </c>
@@ -2691,19 +2534,15 @@
       <c r="I40" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="J40" s="0"/>
-      <c r="K40" s="0"/>
       <c r="L40" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M40" s="0"/>
       <c r="O40" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P40" s="4"/>
-      <c r="Q40" s="0"/>
-    </row>
-    <row r="41" s="5" customFormat="true" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="41" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
         <v>16</v>
       </c>
@@ -2716,7 +2555,6 @@
       <c r="D41" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E41" s="0"/>
       <c r="F41" s="4" t="s">
         <v>112</v>
       </c>
@@ -2732,7 +2570,6 @@
       <c r="J41" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="K41" s="0"/>
       <c r="L41" s="8" t="s">
         <v>113</v>
       </c>
@@ -2745,7 +2582,7 @@
       <c r="P41" s="4"/>
       <c r="Q41" s="6"/>
     </row>
-    <row r="42" s="5" customFormat="true" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
         <v>16</v>
       </c>
@@ -2758,11 +2595,9 @@
       <c r="D42" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E42" s="0"/>
       <c r="F42" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="G42" s="0"/>
       <c r="H42" s="4" t="s">
         <v>114</v>
       </c>
@@ -2772,7 +2607,6 @@
       <c r="J42" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="K42" s="0"/>
       <c r="L42" s="4" t="s">
         <v>37</v>
       </c>
@@ -2783,9 +2617,8 @@
         <v>10</v>
       </c>
       <c r="P42" s="4"/>
-      <c r="Q42" s="0"/>
-    </row>
-    <row r="43" s="5" customFormat="true" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="43" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
         <v>16</v>
       </c>
@@ -2798,11 +2631,9 @@
       <c r="D43" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E43" s="0"/>
       <c r="F43" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="G43" s="0"/>
       <c r="H43" s="4" t="s">
         <v>116</v>
       </c>
@@ -2812,18 +2643,15 @@
       <c r="J43" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="K43" s="0"/>
       <c r="L43" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M43" s="0"/>
       <c r="O43" s="4" t="n">
         <v>5</v>
       </c>
       <c r="P43" s="4"/>
-      <c r="Q43" s="0"/>
-    </row>
-    <row r="44" s="5" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="44" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
         <v>16</v>
       </c>
@@ -2833,33 +2661,28 @@
       <c r="C44" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D44" s="0"/>
       <c r="E44" s="4" t="s">
         <v>55</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="G44" s="0"/>
       <c r="H44" s="4" t="s">
         <v>118</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J44" s="0"/>
       <c r="K44" s="4" t="s">
         <v>120</v>
       </c>
       <c r="L44" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M44" s="0"/>
       <c r="O44" s="4" t="n">
         <v>20</v>
       </c>
       <c r="P44" s="4"/>
-      <c r="Q44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
@@ -3735,13 +3558,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2793522267206"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.89068825910931"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6396761133603"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
@@ -3776,7 +3599,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
         <v>50</v>
       </c>
@@ -3790,7 +3613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
         <v>52</v>
       </c>
@@ -3803,12 +3626,11 @@
       <c r="E3" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="H3" s="0"/>
       <c r="I3" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="4" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
         <v>52</v>
       </c>
@@ -3821,12 +3643,11 @@
       <c r="E4" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="H4" s="0"/>
       <c r="I4" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
         <v>52</v>
       </c>
@@ -3839,12 +3660,11 @@
       <c r="E5" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="H5" s="0"/>
       <c r="I5" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
         <v>52</v>
       </c>
@@ -3857,12 +3677,11 @@
       <c r="E6" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="H6" s="0"/>
       <c r="I6" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="7" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
         <v>52</v>
       </c>
@@ -3875,12 +3694,11 @@
       <c r="E7" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="H7" s="0"/>
       <c r="I7" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="8" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
         <v>52</v>
       </c>
@@ -3893,12 +3711,11 @@
       <c r="E8" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="H8" s="0"/>
       <c r="I8" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="9" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
         <v>74</v>
       </c>
@@ -3908,14 +3725,12 @@
       <c r="C9" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="E9" s="0"/>
       <c r="F9" s="12"/>
-      <c r="H9" s="0"/>
       <c r="I9" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="10" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
         <v>74</v>
       </c>
@@ -3925,14 +3740,12 @@
       <c r="C10" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="E10" s="0"/>
       <c r="F10" s="12"/>
-      <c r="H10" s="0"/>
       <c r="I10" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="11" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
         <v>74</v>
       </c>
@@ -3942,14 +3755,12 @@
       <c r="C11" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="E11" s="0"/>
       <c r="F11" s="12"/>
-      <c r="H11" s="0"/>
       <c r="I11" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="12" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
         <v>74</v>
       </c>
@@ -3959,14 +3770,12 @@
       <c r="C12" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="E12" s="0"/>
       <c r="F12" s="12"/>
-      <c r="H12" s="0"/>
       <c r="I12" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="13" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
         <v>74</v>
       </c>
@@ -3976,14 +3785,12 @@
       <c r="C13" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="E13" s="0"/>
       <c r="F13" s="12"/>
-      <c r="H13" s="0"/>
       <c r="I13" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="14" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
         <v>76</v>
       </c>
@@ -3999,13 +3806,13 @@
       <c r="F14" s="12" t="n">
         <v>12</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
       <c r="I14" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="15" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
         <v>85</v>
       </c>
@@ -4015,15 +3822,12 @@
       <c r="C15" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="E15" s="0"/>
       <c r="F15" s="12"/>
-      <c r="G15" s="0"/>
-      <c r="H15" s="0"/>
       <c r="I15" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="16" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
         <v>85</v>
       </c>
@@ -4033,15 +3837,12 @@
       <c r="C16" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="E16" s="0"/>
       <c r="F16" s="12"/>
-      <c r="G16" s="0"/>
-      <c r="H16" s="0"/>
       <c r="I16" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="17" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
         <v>85</v>
       </c>
@@ -4051,148 +3852,120 @@
       <c r="C17" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="E17" s="0"/>
       <c r="F17" s="12"/>
-      <c r="G17" s="0"/>
-      <c r="H17" s="0"/>
       <c r="I17" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="18" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15" t="s">
+    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="E18" s="0"/>
-      <c r="F18" s="0"/>
-      <c r="G18" s="0"/>
-      <c r="H18" s="0"/>
-      <c r="I18" s="15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="s">
+      <c r="I18" s="14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="E19" s="0"/>
-      <c r="F19" s="0"/>
-      <c r="G19" s="0"/>
-      <c r="H19" s="0"/>
-      <c r="I19" s="15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="s">
+      <c r="I19" s="14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="C20" s="0"/>
-      <c r="E20" s="0"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15" t="s">
+      <c r="F20" s="14"/>
+      <c r="G20" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="H20" s="0"/>
-      <c r="I20" s="15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15" t="s">
+      <c r="I20" s="14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="E21" s="15" t="n">
+      <c r="E21" s="14" t="n">
         <v>18.5</v>
       </c>
-      <c r="F21" s="15"/>
-      <c r="G21" s="0"/>
-      <c r="H21" s="0"/>
-      <c r="I21" s="15" t="n">
+      <c r="F21" s="14"/>
+      <c r="I21" s="14" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="22" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="s">
+    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="C22" s="0"/>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="E22" s="15" t="n">
+      <c r="E22" s="14" t="n">
         <v>20</v>
       </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="0"/>
-      <c r="H22" s="0"/>
-      <c r="I22" s="15" t="n">
+      <c r="F22" s="14"/>
+      <c r="I22" s="14" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="23" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15" t="s">
+    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="C23" s="0"/>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="E23" s="0"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="0"/>
-      <c r="H23" s="0"/>
-      <c r="I23" s="15" t="n">
+      <c r="F23" s="14"/>
+      <c r="I23" s="14" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="24" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C24" s="0"/>
       <c r="D24" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="E24" s="0"/>
-      <c r="F24" s="0"/>
-      <c r="G24" s="0"/>
-      <c r="H24" s="0"/>
       <c r="I24" s="12" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="25" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="12" t="s">
         <v>114</v>
       </c>
@@ -4202,18 +3975,14 @@
       <c r="C25" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="D25" s="0"/>
       <c r="E25" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="F25" s="0"/>
-      <c r="G25" s="0"/>
-      <c r="H25" s="0"/>
       <c r="I25" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="26" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="s">
         <v>114</v>
       </c>
@@ -4223,18 +3992,14 @@
       <c r="C26" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="D26" s="0"/>
       <c r="E26" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="F26" s="0"/>
-      <c r="G26" s="0"/>
-      <c r="H26" s="0"/>
       <c r="I26" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="27" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="12" t="s">
         <v>114</v>
       </c>
@@ -4244,18 +4009,14 @@
       <c r="C27" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="D27" s="0"/>
       <c r="E27" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="F27" s="0"/>
-      <c r="G27" s="0"/>
-      <c r="H27" s="0"/>
       <c r="I27" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="28" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
         <v>114</v>
       </c>
@@ -4265,18 +4026,14 @@
       <c r="C28" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="D28" s="0"/>
       <c r="E28" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="F28" s="0"/>
-      <c r="G28" s="0"/>
-      <c r="H28" s="0"/>
       <c r="I28" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="29" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
         <v>114</v>
       </c>
@@ -4286,18 +4043,14 @@
       <c r="C29" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="D29" s="0"/>
       <c r="E29" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="F29" s="0"/>
-      <c r="G29" s="0"/>
-      <c r="H29" s="0"/>
       <c r="I29" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="30" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
         <v>114</v>
       </c>
@@ -4307,18 +4060,14 @@
       <c r="C30" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="D30" s="0"/>
       <c r="E30" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="F30" s="0"/>
-      <c r="G30" s="0"/>
-      <c r="H30" s="0"/>
       <c r="I30" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="31" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="12" t="s">
         <v>128</v>
       </c>
@@ -4328,16 +4077,11 @@
       <c r="C31" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="D31" s="0"/>
-      <c r="E31" s="0"/>
-      <c r="F31" s="0"/>
-      <c r="G31" s="0"/>
-      <c r="H31" s="0"/>
       <c r="I31" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="32" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="s">
         <v>128</v>
       </c>
@@ -4347,16 +4091,11 @@
       <c r="C32" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="D32" s="0"/>
-      <c r="E32" s="0"/>
-      <c r="F32" s="0"/>
-      <c r="G32" s="0"/>
-      <c r="H32" s="0"/>
       <c r="I32" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="33" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="s">
         <v>128</v>
       </c>
@@ -4366,16 +4105,11 @@
       <c r="C33" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="D33" s="0"/>
-      <c r="E33" s="0"/>
-      <c r="F33" s="0"/>
-      <c r="G33" s="0"/>
-      <c r="H33" s="0"/>
       <c r="I33" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="34" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="s">
         <v>128</v>
       </c>
@@ -4385,16 +4119,11 @@
       <c r="C34" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="D34" s="0"/>
-      <c r="E34" s="0"/>
-      <c r="F34" s="0"/>
-      <c r="G34" s="0"/>
-      <c r="H34" s="0"/>
       <c r="I34" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="35" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="12" t="s">
         <v>128</v>
       </c>
@@ -4404,16 +4133,11 @@
       <c r="C35" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="D35" s="0"/>
-      <c r="E35" s="0"/>
-      <c r="F35" s="0"/>
-      <c r="G35" s="0"/>
-      <c r="H35" s="0"/>
       <c r="I35" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="36" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="12" t="s">
         <v>130</v>
       </c>
@@ -4423,18 +4147,14 @@
       <c r="C36" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="D36" s="0"/>
-      <c r="E36" s="0"/>
       <c r="F36" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="G36" s="0"/>
-      <c r="H36" s="0"/>
       <c r="I36" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="37" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="12" t="s">
         <v>130</v>
       </c>
@@ -4444,18 +4164,14 @@
       <c r="C37" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="D37" s="0"/>
-      <c r="E37" s="0"/>
       <c r="F37" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="G37" s="0"/>
-      <c r="H37" s="0"/>
       <c r="I37" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="38" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="12" t="s">
         <v>130</v>
       </c>
@@ -4465,18 +4181,14 @@
       <c r="C38" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="D38" s="0"/>
       <c r="E38" s="12" t="n">
         <v>64</v>
       </c>
-      <c r="F38" s="0"/>
-      <c r="G38" s="0"/>
-      <c r="H38" s="0"/>
       <c r="I38" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="39" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="12" t="s">
         <v>130</v>
       </c>
@@ -4486,18 +4198,14 @@
       <c r="C39" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="D39" s="0"/>
       <c r="E39" s="12" t="n">
         <v>59</v>
       </c>
-      <c r="F39" s="0"/>
-      <c r="G39" s="0"/>
-      <c r="H39" s="0"/>
       <c r="I39" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="40" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="12" t="s">
         <v>133</v>
       </c>
@@ -4507,16 +4215,11 @@
       <c r="C40" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="D40" s="0"/>
-      <c r="E40" s="0"/>
-      <c r="F40" s="0"/>
-      <c r="G40" s="0"/>
-      <c r="H40" s="0"/>
       <c r="I40" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="41" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="12" t="s">
         <v>135</v>
       </c>
@@ -4526,18 +4229,16 @@
       <c r="C41" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="D41" s="0"/>
       <c r="E41" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="F41" s="0"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
       <c r="I41" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="42" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="s">
         <v>135</v>
       </c>
@@ -4547,25 +4248,22 @@
       <c r="C42" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="D42" s="0"/>
       <c r="E42" s="12" t="n">
         <v>33.8</v>
       </c>
-      <c r="F42" s="0"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
       <c r="I42" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="43" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="12" t="s">
         <v>100</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C43" s="0"/>
       <c r="D43" s="12" t="s">
         <v>196</v>
       </c>
@@ -4575,20 +4273,17 @@
       <c r="F43" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="G43" s="0"/>
-      <c r="H43" s="0"/>
       <c r="I43" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="44" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="s">
         <v>100</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C44" s="0"/>
       <c r="D44" s="12" t="s">
         <v>196</v>
       </c>
@@ -4598,51 +4293,39 @@
       <c r="F44" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="G44" s="0"/>
-      <c r="H44" s="0"/>
       <c r="I44" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="45" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="12" t="s">
         <v>102</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="D45" s="0"/>
-      <c r="E45" s="0"/>
-      <c r="F45" s="0"/>
-      <c r="G45" s="0"/>
-      <c r="H45" s="0"/>
       <c r="I45" s="12" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="46" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="16" t="s">
         <v>198</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="D46" s="0"/>
-      <c r="E46" s="0"/>
-      <c r="F46" s="0"/>
-      <c r="G46" s="0"/>
-      <c r="H46" s="0"/>
       <c r="I46" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="47" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="s">
         <v>157</v>
       </c>
@@ -4652,16 +4335,11 @@
       <c r="C47" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="D47" s="0"/>
-      <c r="E47" s="0"/>
-      <c r="F47" s="0"/>
-      <c r="G47" s="0"/>
-      <c r="H47" s="0"/>
       <c r="I47" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="48" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="s">
         <v>157</v>
       </c>
@@ -4671,16 +4349,11 @@
       <c r="C48" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="D48" s="0"/>
-      <c r="E48" s="0"/>
-      <c r="F48" s="0"/>
-      <c r="G48" s="0"/>
-      <c r="H48" s="0"/>
       <c r="I48" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="49" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="12" t="s">
         <v>157</v>
       </c>
@@ -4690,16 +4363,11 @@
       <c r="C49" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="D49" s="0"/>
-      <c r="E49" s="0"/>
-      <c r="F49" s="0"/>
-      <c r="G49" s="0"/>
-      <c r="H49" s="0"/>
       <c r="I49" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="50" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="12" t="s">
         <v>157</v>
       </c>
@@ -4709,16 +4377,11 @@
       <c r="C50" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="D50" s="0"/>
-      <c r="E50" s="0"/>
-      <c r="F50" s="0"/>
-      <c r="G50" s="0"/>
-      <c r="H50" s="0"/>
       <c r="I50" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="51" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="12" t="s">
         <v>157</v>
       </c>
@@ -4728,100 +4391,79 @@
       <c r="C51" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="D51" s="0"/>
-      <c r="E51" s="0"/>
-      <c r="F51" s="0"/>
-      <c r="G51" s="0"/>
-      <c r="H51" s="0"/>
       <c r="I51" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="52" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="16" t="s">
         <v>198</v>
       </c>
       <c r="C52" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="D52" s="0"/>
-      <c r="E52" s="0"/>
       <c r="F52" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="G52" s="0"/>
-      <c r="H52" s="0"/>
       <c r="I52" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="53" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="16" t="s">
         <v>198</v>
       </c>
       <c r="C53" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="D53" s="0"/>
-      <c r="E53" s="0"/>
       <c r="F53" s="12" t="n">
         <v>10</v>
       </c>
-      <c r="G53" s="0"/>
-      <c r="H53" s="0"/>
       <c r="I53" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="54" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="16" t="s">
         <v>198</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="D54" s="0"/>
-      <c r="E54" s="0"/>
       <c r="F54" s="12" t="n">
         <v>12</v>
       </c>
-      <c r="G54" s="0"/>
-      <c r="H54" s="0"/>
       <c r="I54" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="55" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="16" t="s">
         <v>198</v>
       </c>
       <c r="C55" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="D55" s="0"/>
-      <c r="E55" s="0"/>
       <c r="F55" s="12" t="n">
         <v>24</v>
       </c>
-      <c r="G55" s="0"/>
-      <c r="H55" s="0"/>
       <c r="I55" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="56" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="12" t="s">
         <v>169</v>
       </c>
@@ -4831,18 +4473,14 @@
       <c r="C56" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="D56" s="0"/>
       <c r="E56" s="12" t="n">
         <v>18.5</v>
       </c>
-      <c r="F56" s="0"/>
-      <c r="G56" s="0"/>
-      <c r="H56" s="0"/>
       <c r="I56" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="57" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="12" t="s">
         <v>171</v>
       </c>
@@ -4852,18 +4490,16 @@
       <c r="C57" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="D57" s="0"/>
       <c r="E57" s="12" t="n">
         <v>23.7</v>
       </c>
-      <c r="F57" s="0"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
       <c r="I57" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="58" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="12" t="s">
         <v>171</v>
       </c>
@@ -4873,18 +4509,16 @@
       <c r="C58" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="D58" s="0"/>
       <c r="E58" s="12" t="n">
         <v>33.8</v>
       </c>
-      <c r="F58" s="0"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
       <c r="I58" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="59" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="12" t="s">
         <v>139</v>
       </c>
@@ -4894,18 +4528,16 @@
       <c r="C59" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="D59" s="0"/>
       <c r="E59" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="F59" s="0"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
       <c r="I59" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="60" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="12" t="s">
         <v>139</v>
       </c>
@@ -4915,25 +4547,22 @@
       <c r="C60" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="D60" s="0"/>
       <c r="E60" s="12" t="n">
         <v>33.8</v>
       </c>
-      <c r="F60" s="0"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
       <c r="I60" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="61" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="12" t="s">
         <v>141</v>
       </c>
       <c r="B61" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C61" s="0"/>
       <c r="D61" s="12" t="s">
         <v>196</v>
       </c>
@@ -4943,20 +4572,17 @@
       <c r="F61" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="G61" s="0"/>
-      <c r="H61" s="0"/>
       <c r="I61" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="62" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="12" t="s">
         <v>141</v>
       </c>
       <c r="B62" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C62" s="0"/>
       <c r="D62" s="12" t="s">
         <v>196</v>
       </c>
@@ -4966,13 +4592,11 @@
       <c r="F62" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="G62" s="0"/>
-      <c r="H62" s="0"/>
       <c r="I62" s="12" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="63" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="12" t="s">
         <v>143</v>
       </c>
@@ -4982,11 +4606,6 @@
       <c r="C63" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="D63" s="0"/>
-      <c r="E63" s="0"/>
-      <c r="F63" s="0"/>
-      <c r="G63" s="0"/>
-      <c r="H63" s="0"/>
       <c r="I63" s="12" t="n">
         <v>2</v>
       </c>
@@ -5010,22 +4629,22 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="L22" activeCellId="0" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.67611336032389"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.9230769230769"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
@@ -5035,40 +4654,40 @@
       <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="17" t="s">
         <v>213</v>
       </c>
     </row>
@@ -5094,6 +4713,9 @@
       <c r="K2" s="0" t="s">
         <v>217</v>
       </c>
+      <c r="L2" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -5123,6 +4745,9 @@
       <c r="K3" s="0" t="s">
         <v>220</v>
       </c>
+      <c r="L3" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -5146,6 +4771,9 @@
       <c r="K4" s="0" t="s">
         <v>217</v>
       </c>
+      <c r="L4" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -5163,7 +4791,7 @@
       <c r="E5" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>221</v>
       </c>
       <c r="G5" s="0" t="s">
@@ -5174,6 +4802,9 @@
       </c>
       <c r="K5" s="0" t="s">
         <v>220</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5198,6 +4829,9 @@
       <c r="K6" s="0" t="s">
         <v>217</v>
       </c>
+      <c r="L6" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -5227,6 +4861,9 @@
       <c r="K7" s="0" t="s">
         <v>220</v>
       </c>
+      <c r="L7" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -5276,6 +4913,9 @@
       <c r="K9" s="0" t="s">
         <v>217</v>
       </c>
+      <c r="L9" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -5305,6 +4945,9 @@
       <c r="K10" s="0" t="s">
         <v>220</v>
       </c>
+      <c r="L10" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -5328,6 +4971,9 @@
       <c r="K11" s="0" t="s">
         <v>217</v>
       </c>
+      <c r="L11" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -5357,6 +5003,9 @@
       <c r="K12" s="0" t="s">
         <v>220</v>
       </c>
+      <c r="L12" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -5380,6 +5029,9 @@
       <c r="K13" s="0" t="s">
         <v>217</v>
       </c>
+      <c r="L13" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -5409,6 +5061,9 @@
       <c r="K14" s="0" t="s">
         <v>220</v>
       </c>
+      <c r="L14" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -5432,6 +5087,9 @@
       <c r="K15" s="0" t="s">
         <v>217</v>
       </c>
+      <c r="L15" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -5455,6 +5113,9 @@
       <c r="K16" s="0" t="s">
         <v>217</v>
       </c>
+      <c r="L16" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -5478,6 +5139,9 @@
       <c r="K17" s="0" t="s">
         <v>217</v>
       </c>
+      <c r="L17" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -5501,6 +5165,9 @@
       <c r="K18" s="0" t="s">
         <v>217</v>
       </c>
+      <c r="L18" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
@@ -5530,6 +5197,9 @@
       <c r="K19" s="0" t="s">
         <v>220</v>
       </c>
+      <c r="L19" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -5553,6 +5223,9 @@
       <c r="K20" s="0" t="s">
         <v>217</v>
       </c>
+      <c r="L20" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
@@ -5582,7 +5255,10 @@
       <c r="K21" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="M21" s="20" t="s">
+      <c r="L21" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="M21" s="18" t="s">
         <v>227</v>
       </c>
     </row>
@@ -5607,6 +5283,9 @@
       </c>
       <c r="K22" s="0" t="s">
         <v>217</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -5627,50 +5306,50 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.60728744939271"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.9230769230769"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.2388663967611"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="20" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5678,13 +5357,15 @@
       <c r="A2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="I2" s="0" t="n">
         <v>80</v>
       </c>
@@ -5699,6 +5380,9 @@
       <c r="G3" s="0" t="s">
         <v>229</v>
       </c>
+      <c r="H3" s="0" t="s">
+        <v>32</v>
+      </c>
       <c r="I3" s="0" t="n">
         <v>80</v>
       </c>
@@ -5710,14 +5394,16 @@
       <c r="F4" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="H4" s="24"/>
+      <c r="H4" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="I4" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="J4" s="25"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -5729,6 +5415,9 @@
       <c r="G5" s="0" t="s">
         <v>182</v>
       </c>
+      <c r="H5" s="0" t="s">
+        <v>32</v>
+      </c>
       <c r="I5" s="0" t="n">
         <v>80</v>
       </c>
@@ -5737,19 +5426,19 @@
       <c r="A6" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="24" t="s">
         <v>231</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="27" t="n">
+      <c r="I6" s="25" t="n">
         <v>100</v>
       </c>
-      <c r="J6" s="25"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -5758,13 +5447,16 @@
       <c r="F7" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="I7" s="27" t="n">
+      <c r="H7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="25" t="n">
         <v>51</v>
       </c>
-      <c r="J7" s="25"/>
+      <c r="J7" s="23"/>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -5776,6 +5468,9 @@
       <c r="G8" s="0" t="s">
         <v>182</v>
       </c>
+      <c r="H8" s="0" t="s">
+        <v>32</v>
+      </c>
       <c r="I8" s="0" t="n">
         <v>80</v>
       </c>
@@ -5789,6 +5484,9 @@
       </c>
       <c r="G9" s="0" t="s">
         <v>182</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>80</v>
@@ -5819,454 +5517,445 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="91.8016194331984"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.3481781376518"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="2" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="C2" s="13" t="n">
+      <c r="C2" s="0" t="n">
         <v>114</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="0" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="3" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="C3" s="13" t="n">
+      <c r="C3" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="0" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="4" s="13" customFormat="true" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="s">
+    <row r="4" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="C4" s="20" t="n">
+      <c r="C4" s="18" t="n">
         <v>141</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="C5" s="13" t="n">
+      <c r="C5" s="0" t="n">
         <v>86</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="6" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="C6" s="13" t="n">
+      <c r="C6" s="0" t="n">
         <v>86</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="7" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="C7" s="13" t="n">
+      <c r="C7" s="0" t="n">
         <v>86</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="8" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="C8" s="13" t="n">
+      <c r="C8" s="0" t="n">
         <v>83</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E8" s="0"/>
-    </row>
-    <row r="9" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="C9" s="13" t="n">
+      <c r="C9" s="0" t="n">
         <v>84</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E9" s="0"/>
-    </row>
-    <row r="10" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="C10" s="13" t="n">
+      <c r="C10" s="0" t="n">
         <v>89</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E10" s="0"/>
-    </row>
-    <row r="11" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="C11" s="13" t="n">
+      <c r="C11" s="0" t="n">
         <v>88</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E11" s="0"/>
-    </row>
-    <row r="12" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="C12" s="13" t="n">
+      <c r="C12" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E12" s="0"/>
-    </row>
-    <row r="13" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="C13" s="13" t="n">
+      <c r="C13" s="0" t="n">
         <v>87</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="14" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="s">
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="C14" s="13" t="n">
+      <c r="C14" s="0" t="n">
         <v>87</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="15" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="s">
+    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="C15" s="13" t="n">
+      <c r="C15" s="0" t="n">
         <v>98</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="16" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="s">
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="C16" s="13" t="n">
+      <c r="C16" s="0" t="n">
         <v>99</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E16" s="0"/>
-    </row>
-    <row r="17" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="C17" s="13" t="n">
+      <c r="C17" s="0" t="n">
         <v>123</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="E17" s="0"/>
-    </row>
-    <row r="18" s="13" customFormat="true" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="C18" s="20" t="n">
+      <c r="C18" s="18" t="n">
         <v>137</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="E18" s="20"/>
-    </row>
-    <row r="19" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
+      <c r="E18" s="18"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="C19" s="13" t="n">
+      <c r="C19" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="20" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="s">
+    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="C20" s="13" t="n">
+      <c r="C20" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="21" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="s">
+    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="C21" s="13" t="n">
+      <c r="C21" s="0" t="n">
         <v>98</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="22" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13" t="s">
+    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="C22" s="13" t="n">
+      <c r="C22" s="0" t="n">
         <v>123</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="E22" s="0"/>
-    </row>
-    <row r="23" s="13" customFormat="true" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="C23" s="20" t="n">
+      <c r="C23" s="18" t="n">
         <v>134</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="E23" s="20"/>
-    </row>
-    <row r="24" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13" t="s">
+      <c r="E23" s="18"/>
+    </row>
+    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="C24" s="13" t="n">
+      <c r="C24" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E24" s="0"/>
-    </row>
-    <row r="25" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="20" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="C25" s="20" t="n">
+      <c r="C25" s="18" t="n">
         <v>110</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="18" t="s">
         <v>246</v>
       </c>
-      <c r="E25" s="20"/>
-    </row>
-    <row r="26" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13" t="s">
+      <c r="E25" s="18"/>
+    </row>
+    <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="C26" s="13" t="n">
+      <c r="C26" s="0" t="n">
         <v>118</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="27" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="13" t="s">
+    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="C27" s="13" t="n">
+      <c r="C27" s="0" t="n">
         <v>118</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="28" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="13" t="s">
+    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="C28" s="13" t="n">
+      <c r="C28" s="0" t="n">
         <v>118</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="0" t="s">
         <v>242</v>
       </c>
     </row>
@@ -6286,59 +5975,223 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.8623481781377"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.2753036437247"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.3117408906883"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.6315789473684"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="20" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>80</v>
       </c>
+      <c r="D2" s="24" t="s">
+        <v>268</v>
+      </c>
       <c r="F2" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="61.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="28" t="s">
-        <v>269</v>
-      </c>
-    </row>
+      <c r="D3" s="24" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -6364,29 +6217,29 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
-        <v>270</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>271</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>267</v>
@@ -6394,23 +6247,23 @@
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>215</v>
@@ -6418,7 +6271,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>214</v>
@@ -6426,7 +6279,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>215</v>
@@ -6442,10 +6295,10 @@
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fixed template for CR&LT11 to run before CR&LT10
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS/Data/KPITemplateV4.6.xlsx
+++ b/Projects/CCBOTTLERSUS/Data/KPITemplateV4.6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,6 +21,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$I$63</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Survey!$A$1:$E$28</definedName>
   </definedNames>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="284">
   <si>
     <t xml:space="preserve">Region</t>
   </si>
@@ -1215,29 +1216,29 @@
   </sheetPr>
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6396761133603"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.3886639676113"/>
@@ -1330,7 +1331,7 @@
       </c>
       <c r="P2" s="4"/>
     </row>
-    <row r="3" s="5" customFormat="true" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1343,16 +1344,18 @@
       <c r="D3" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="E3" s="5"/>
       <c r="F3" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="G3" s="5"/>
       <c r="H3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="0"/>
+      <c r="J3" s="5"/>
       <c r="L3" s="4" t="s">
         <v>23</v>
       </c>
@@ -1362,7 +1365,7 @@
       </c>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" s="5" customFormat="true" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1384,7 +1387,9 @@
       <c r="I4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="0"/>
+      <c r="K4" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="L4" s="4" t="s">
         <v>23</v>
       </c>
@@ -3558,13 +3563,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1781376518219"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.89068825910931"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
@@ -4636,15 +4641,15 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.67611336032389"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.7773279352227"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
@@ -5314,11 +5319,11 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.60728744939271"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.2388663967611"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.5627530364373"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
@@ -5517,10 +5522,10 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.8866396761134"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5977,18 +5982,18 @@
   </sheetPr>
   <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.5951417004049"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.6315789473684"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.0607287449393"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6217,7 +6222,7 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>